<commit_message>
SCM002: add SRS document
</commit_message>
<xml_diff>
--- a/01 Inception/01 Baseline/SCMBlog_Estimation v1.0.xlsx
+++ b/01 Inception/01 Baseline/SCMBlog_Estimation v1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\OJT\SCM\DummyProject\scmtraining\01 Inception\02 Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\OJT\SCM\DummyProject\scmtraining\01 Inception\01 Baseline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Edi Prayitno</t>
+  </si>
+  <si>
+    <t>Update as Baseline document</t>
   </si>
 </sst>
 </file>
@@ -251,13 +254,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,90 +546,98 @@
   <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.25" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>42648</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>0.1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="7">
+        <v>42653</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>